<commit_message>
Version 0.1.1.9 - The price tag format editor has been fully implemented, and the interface has been improved, making it more modern and concise
</commit_message>
<xml_diff>
--- a/docs/OtherHelpfulFiles/Для тесту!.xlsx
+++ b/docs/OtherHelpfulFiles/Для тесту!.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Psina\Desktop\AlexWork\AppProjects\PriceTagMasterProject_ver2\docs\OtherHelpfulFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sekin-novikov\Desktop\WorkFiles\OtherProjects\PriceTagMasterProject_ver2\docs\OtherHelpfulFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C4BA04-88BF-4CB4-812C-DFA1ABCDFB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19590" yWindow="2490" windowWidth="25710" windowHeight="18510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21690" yWindow="2490" windowWidth="25710" windowHeight="18510"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
   <si>
     <t>Поставщик</t>
   </si>
@@ -129,12 +128,6 @@
     <t>Количество</t>
   </si>
   <si>
-    <t>муж 9</t>
-  </si>
-  <si>
-    <t>жен 7,2</t>
-  </si>
-  <si>
     <t>г. Москва, ул.Малая Бобровская,д.18, кв.62</t>
   </si>
   <si>
@@ -162,12 +155,6 @@
     <t>Кольцо</t>
   </si>
   <si>
-    <t>муж 22</t>
-  </si>
-  <si>
-    <t>муж 8</t>
-  </si>
-  <si>
     <t>Германия</t>
   </si>
   <si>
@@ -187,12 +174,15 @@
   </si>
   <si>
     <t>ASDW3123</t>
+  </si>
+  <si>
+    <t>жен</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -788,11 +778,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,7 +881,7 @@
         <v>1493</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>19</v>
@@ -915,7 +905,7 @@
         <v>2540</v>
       </c>
       <c r="O4" s="20">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>15</v>
@@ -938,7 +928,7 @@
         <v>748</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>19</v>
@@ -949,8 +939,8 @@
       <c r="J5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>13</v>
+      <c r="K5" s="2">
+        <v>3</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>23</v>
@@ -1019,16 +1009,16 @@
         <v>16</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F7" s="9">
         <v>748</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>29</v>
@@ -1039,11 +1029,11 @@
       <c r="J7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>13</v>
+      <c r="K7" s="2">
+        <v>7.5</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="M7" s="2">
         <v>4234</v>
@@ -1052,7 +1042,7 @@
         <v>568</v>
       </c>
       <c r="O7" s="21">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>27</v>
@@ -1065,13 +1055,13 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F8" s="9">
         <v>3</v>
@@ -1080,19 +1070,19 @@
         <v>17</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="M8" s="2">
         <v>6765</v>
@@ -1115,16 +1105,16 @@
         <v>16</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F9" s="9">
         <v>675</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>29</v>
@@ -1135,11 +1125,11 @@
       <c r="J9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>13</v>
+      <c r="K9" s="2">
+        <v>2</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M9" s="2">
         <v>332</v>
@@ -1162,10 +1152,10 @@
         <v>16</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F10" s="9">
         <v>453</v>
@@ -1174,19 +1164,19 @@
         <v>17</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>13</v>
+      <c r="K10" s="2">
+        <v>18</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="M10" s="2">
         <v>1890</v>

</xml_diff>